<commit_message>
Project-Defect Report for E-commerce website
Project-Defect report For LUMA E-commerce Websites use bug Tracking tool by Bugzilla.
</commit_message>
<xml_diff>
--- a/Defectproject/testcasesforLUMA.xlsx
+++ b/Defectproject/testcasesforLUMA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7365" windowWidth="14295" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="7365" windowWidth="14295" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Testcase-1" sheetId="1" r:id="rId1"/>
@@ -3882,7 +3882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="12" customFormat="1" ht="351">
+    <row r="45" spans="1:10" s="12" customFormat="1" ht="324">
       <c r="A45" s="16">
         <v>43</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="12" customFormat="1" ht="351">
+    <row r="46" spans="1:10" s="12" customFormat="1" ht="324">
       <c r="A46" s="16">
         <v>44</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="12" customFormat="1" ht="351">
+    <row r="47" spans="1:10" s="12" customFormat="1" ht="324">
       <c r="A47" s="16">
         <v>45</v>
       </c>
@@ -8729,8 +8729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12673,8 +12673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30"/>

</xml_diff>